<commit_message>
Avances del proyecto final de econometría
</commit_message>
<xml_diff>
--- a/materias/Seminario de economía/organizar la data/data.xlsx
+++ b/materias/Seminario de economía/organizar la data/data.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JoseA\OneDrive\Escritorio\rstudio_projects\maestria-economia\materias\Seminario de economía\organizar la data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{68ADD838-79FC-489D-9821-05605D758A8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D6419DC-A39F-4208-832E-19325CDAFE7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{13E0D3F0-C389-4DD7-857A-6919231AA570}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="2" r:id="rId1"/>
-    <sheet name="var" sheetId="4" r:id="rId2"/>
+    <sheet name="vars" sheetId="4" r:id="rId2"/>
     <sheet name="diccionario" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -130,8 +130,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -178,8 +178,8 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>

</xml_diff>